<commit_message>
clients api, urls updated
</commit_message>
<xml_diff>
--- a/EconomicServlet/url.xlsx
+++ b/EconomicServlet/url.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="LOCAL_DATE_SEPARATOR" vbProcedure="false">NA()</definedName>
-    <definedName function="false" hidden="false" name="LOCAL_DAY_FORMAT" vbProcedure="false">NA()</definedName>
-    <definedName function="false" hidden="false" name="LOCAL_HOUR_FORMAT" vbProcedure="false">NA()</definedName>
-    <definedName function="false" hidden="false" name="LOCAL_MINUTE_FORMAT" vbProcedure="false">NA()</definedName>
-    <definedName function="false" hidden="false" name="LOCAL_MONTH_FORMAT" vbProcedure="false">NA()</definedName>
-    <definedName function="false" hidden="false" name="LOCAL_MYSQL_DATE_FORMAT" vbProcedure="false">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName function="false" hidden="false" name="LOCAL_YEAR_FORMAT" vbProcedure="false">NA()</definedName>
-    <definedName function="false" hidden="false" name="LOCAL_TIME_SEPARATOR" vbProcedure="false">NA()</definedName>
-    <definedName function="false" hidden="false" name="LOCAL_SECOND_FORMAT" vbProcedure="false">NA()</definedName>
-    <definedName function="false" hidden="false" name="__xlfn_FINV" vbProcedure="false">NA()</definedName>
+    <definedName name="__xlfn_FINV">NA()</definedName>
+    <definedName name="LOCAL_DATE_SEPARATOR">NA()</definedName>
+    <definedName name="LOCAL_DAY_FORMAT">NA()</definedName>
+    <definedName name="LOCAL_HOUR_FORMAT">NA()</definedName>
+    <definedName name="LOCAL_MINUTE_FORMAT">NA()</definedName>
+    <definedName name="LOCAL_MONTH_FORMAT">NA()</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_SECOND_FORMAT">NA()</definedName>
+    <definedName name="LOCAL_TIME_SEPARATOR">NA()</definedName>
+    <definedName name="LOCAL_YEAR_FORMAT">NA()</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
   <si>
     <t>url</t>
   </si>
@@ -58,7 +57,7 @@
     <t>принимает параметры login и password возвращает объект Client</t>
   </si>
   <si>
-    <t> /createOrder</t>
+    <t>/createOrder</t>
   </si>
   <si>
     <t>принимает массив объектов Good, с дополнительным полем number, оформляет заказ</t>
@@ -148,7 +147,7 @@
     <t>/deleteOrder</t>
   </si>
   <si>
-    <t>принимает id заказа и удаляет его </t>
+    <t>принимает id заказа и удаляет его</t>
   </si>
   <si>
     <t>/createRegularOrder</t>
@@ -203,16 +202,16 @@
   </si>
   <si>
     <t>принимает id товара и файл картинки, сохраняет картинку в resources/img и записывает путь к картинке в imagePath товара</t>
+  </si>
+  <si>
+    <t>+/-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="7">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -220,25 +219,7 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -268,7 +249,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -276,83 +257,323 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+  <a:themeElements>
+    <a:clrScheme name="Стандартная">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Стандартная">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Стандартная">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="109.020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0510204081633"/>
+    <col min="1" max="1" width="35.42578125"/>
+    <col min="2" max="2" width="109"/>
+    <col min="4" max="4" width="53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -363,302 +584,316 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="4" t="s">
         <v>51</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="C34" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CСтраница &amp;P</oddFooter>
   </headerFooter>

</xml_diff>